<commit_message>
feat: WorklogWelding 리드탭 필드 확장
</commit_message>
<xml_diff>
--- a/data/templates/worklog/10.Welding.xlsx
+++ b/data/templates/worklog/10.Welding.xlsx
@@ -5,72 +5,78 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\user\Desktop\eurocell-mes-be\data\templates\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\user\Desktop\eurocell-mes-be\data\templates\worklog\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3003E93C-4E57-41E3-999D-EDB362E25F5C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{16DB85A4-40AD-4215-B01A-EA21F2AD740F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-17355" yWindow="210" windowWidth="19140" windowHeight="15210" xr2:uid="{316051C1-BE5C-449C-8818-DF2E3CD47082}"/>
+    <workbookView xWindow="3585" yWindow="705" windowWidth="18735" windowHeight="13965" xr2:uid="{316051C1-BE5C-449C-8818-DF2E3CD47082}"/>
   </bookViews>
   <sheets>
     <sheet name="원본" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
     <definedName name="approver">원본!$L$5</definedName>
-    <definedName name="cleanCheck">원본!$G$44</definedName>
-    <definedName name="equipmentCheckResult">원본!$C$41</definedName>
-    <definedName name="equipmentIssue">원본!$K$41</definedName>
-    <definedName name="hipot2DefectQuantity">원본!$I$27</definedName>
-    <definedName name="hipot2DefectRemark">원본!$J$27</definedName>
-    <definedName name="hipot2GoodQuantity">원본!$G$27</definedName>
-    <definedName name="hipot2JrNumber">원본!$C$27</definedName>
-    <definedName name="hipot2WorkQuantity">원본!$E$27</definedName>
-    <definedName name="hipotTime">원본!$E$39</definedName>
-    <definedName name="hipotVoltage">원본!$C$39</definedName>
-    <definedName name="jigNumber">원본!$G$41</definedName>
+    <definedName name="cleanCheck">원본!$G$46</definedName>
+    <definedName name="equipmentCheckResult">원본!$C$43</definedName>
+    <definedName name="equipmentIssue">원본!$K$43</definedName>
+    <definedName name="hipot2DefectQuantity">원본!$I$29</definedName>
+    <definedName name="hipot2DefectRemark">원본!$J$29</definedName>
+    <definedName name="hipot2GoodQuantity">원본!$G$29</definedName>
+    <definedName name="hipot2JrNumber">원본!$C$29</definedName>
+    <definedName name="hipot2WorkQuantity">원본!$E$29</definedName>
+    <definedName name="hipotTime">원본!$E$41</definedName>
+    <definedName name="hipotVoltage">원본!$C$41</definedName>
+    <definedName name="jigNumber">원본!$G$43</definedName>
+    <definedName name="leadTab2Lot">원본!$C$16</definedName>
+    <definedName name="leadTab2Manufacturer">원본!$E$16</definedName>
+    <definedName name="leadTab2Spec">원본!$G$16</definedName>
+    <definedName name="leadTab2Type">원본!$A$16</definedName>
+    <definedName name="leadTab2Usage">원본!$K$16</definedName>
     <definedName name="leadTabLot">원본!$C$14</definedName>
     <definedName name="leadTabManufacturer">원본!$E$14</definedName>
     <definedName name="leadTabSpec">원본!$G$14</definedName>
+    <definedName name="leadTabType">원본!$A$14</definedName>
     <definedName name="leadTabUsage">원본!$K$14</definedName>
     <definedName name="line">원본!$C$9</definedName>
-    <definedName name="mainWeldingAmplitude">원본!$E$36</definedName>
-    <definedName name="mainWeldingDefectQuantity">원본!$I$24</definedName>
-    <definedName name="mainWeldingDefectRemark">원본!$J$24</definedName>
-    <definedName name="mainWeldingEnergy">원본!$C$36</definedName>
-    <definedName name="mainWeldingGoodQuantity">원본!$G$24</definedName>
-    <definedName name="mainWeldingHoldTime">원본!$K$36</definedName>
-    <definedName name="mainWeldingJrNumber">원본!$C$24</definedName>
-    <definedName name="mainWeldingPressure">원본!$I$36</definedName>
-    <definedName name="mainWeldingStopper">원본!$G$36</definedName>
-    <definedName name="mainWeldingWorkQuantity">원본!$E$24</definedName>
+    <definedName name="mainWeldingAmplitude">원본!$E$38</definedName>
+    <definedName name="mainWeldingDefectQuantity">원본!$I$26</definedName>
+    <definedName name="mainWeldingDefectRemark">원본!$J$26</definedName>
+    <definedName name="mainWeldingEnergy">원본!$C$38</definedName>
+    <definedName name="mainWeldingGoodQuantity">원본!$G$26</definedName>
+    <definedName name="mainWeldingHoldTime">원본!$K$38</definedName>
+    <definedName name="mainWeldingJrNumber">원본!$C$26</definedName>
+    <definedName name="mainWeldingPressure">원본!$I$38</definedName>
+    <definedName name="mainWeldingStopper">원본!$G$38</definedName>
+    <definedName name="mainWeldingWorkQuantity">원본!$E$26</definedName>
     <definedName name="manufactureDate">원본!$C$7</definedName>
-    <definedName name="piTapeLot">원본!$C$16</definedName>
-    <definedName name="piTapeManufacturer">원본!$E$16</definedName>
-    <definedName name="piTapeSpec">원본!$G$16</definedName>
-    <definedName name="piTapeUsage">원본!$K$16</definedName>
+    <definedName name="piTapeLot">원본!$C$18</definedName>
+    <definedName name="piTapeManufacturer">원본!$E$18</definedName>
+    <definedName name="piTapeSpec">원본!$G$18</definedName>
+    <definedName name="piTapeUsage">원본!$K$18</definedName>
     <definedName name="plant">원본!$G$9</definedName>
-    <definedName name="preWeldingAmplitude">원본!$E$34</definedName>
-    <definedName name="preWeldingDefectQuantity">원본!$I$21</definedName>
-    <definedName name="preWeldingDefectRemark">원본!$J$21</definedName>
-    <definedName name="preWeldingEnergy">원본!$C$34</definedName>
-    <definedName name="preWeldingGoodQuantity">원본!$G$21</definedName>
-    <definedName name="preWeldingHoldTime">원본!$K$34</definedName>
-    <definedName name="preWeldingJrNumber">원본!$C$21</definedName>
-    <definedName name="preWeldingPressure">원본!$I$34</definedName>
-    <definedName name="preWeldingStopper">원본!$G$34</definedName>
-    <definedName name="preWeldingWorkQuantity">원본!$E$21</definedName>
+    <definedName name="preWeldingAmplitude">원본!$E$36</definedName>
+    <definedName name="preWeldingDefectQuantity">원본!$I$23</definedName>
+    <definedName name="preWeldingDefectRemark">원본!$J$23</definedName>
+    <definedName name="preWeldingEnergy">원본!$C$36</definedName>
+    <definedName name="preWeldingGoodQuantity">원본!$G$23</definedName>
+    <definedName name="preWeldingHoldTime">원본!$K$36</definedName>
+    <definedName name="preWeldingJrNumber">원본!$C$23</definedName>
+    <definedName name="preWeldingPressure">원본!$I$36</definedName>
+    <definedName name="preWeldingStopper">원본!$G$36</definedName>
+    <definedName name="preWeldingWorkQuantity">원본!$E$23</definedName>
     <definedName name="productionId">원본!$G$7</definedName>
-    <definedName name="remark">원본!$A$47</definedName>
+    <definedName name="remark">원본!$A$49</definedName>
     <definedName name="reviewer">원본!$K$5</definedName>
-    <definedName name="safety">원본!$K$44</definedName>
+    <definedName name="safety">원본!$K$46</definedName>
     <definedName name="shift">원본!$K$9</definedName>
-    <definedName name="tapingDefectQuantity">원본!$I$29</definedName>
-    <definedName name="tapingDefectRemark">원본!$J$29</definedName>
-    <definedName name="tapingGoodQuantity">원본!$G$29</definedName>
-    <definedName name="tapingJrNumber">원본!$C$29</definedName>
-    <definedName name="tapingLength">원본!$I$39</definedName>
-    <definedName name="tapingWorkQuantity">원본!$E$29</definedName>
-    <definedName name="tempHumi">원본!$C$44</definedName>
+    <definedName name="tapingDefectQuantity">원본!$I$31</definedName>
+    <definedName name="tapingDefectRemark">원본!$J$31</definedName>
+    <definedName name="tapingGoodQuantity">원본!$G$31</definedName>
+    <definedName name="tapingJrNumber">원본!$C$31</definedName>
+    <definedName name="tapingLength">원본!$I$41</definedName>
+    <definedName name="tapingWorkQuantity">원본!$E$31</definedName>
+    <definedName name="tempHumi">원본!$C$46</definedName>
     <definedName name="worker">원본!$K$7</definedName>
     <definedName name="writer">원본!$J$5</definedName>
   </definedNames>
@@ -95,7 +101,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="55">
   <si>
     <t>웰딩 작업 일지</t>
     <phoneticPr fontId="3" type="noConversion"/>
@@ -644,110 +650,110 @@
     <xf numFmtId="176" fontId="5" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="1" fontId="5" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="5" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="5" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="5" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="5" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="5" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="11" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="5" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="5" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="5" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="5" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="5" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="5" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="11" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1159,10 +1165,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:L53"/>
+  <dimension ref="A1:L55"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" view="pageBreakPreview" zoomScale="85" zoomScaleNormal="90" zoomScaleSheetLayoutView="85" workbookViewId="0">
-      <selection sqref="A1:I5"/>
+    <sheetView showGridLines="0" tabSelected="1" view="pageBreakPreview" topLeftCell="A7" zoomScale="85" zoomScaleNormal="90" zoomScaleSheetLayoutView="85" workbookViewId="0">
+      <selection activeCell="A16" sqref="A16:B17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -1420,565 +1426,567 @@
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A16" s="8" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B16" s="8"/>
       <c r="C16" s="16"/>
       <c r="D16" s="16"/>
-      <c r="E16" s="16"/>
-      <c r="F16" s="16"/>
-      <c r="G16" s="25"/>
-      <c r="H16" s="26"/>
-      <c r="I16" s="26"/>
-      <c r="J16" s="27"/>
-      <c r="K16" s="16"/>
-      <c r="L16" s="16"/>
+      <c r="E16" s="17"/>
+      <c r="F16" s="17"/>
+      <c r="G16" s="18"/>
+      <c r="H16" s="19"/>
+      <c r="I16" s="19"/>
+      <c r="J16" s="20"/>
+      <c r="K16" s="24"/>
+      <c r="L16" s="24"/>
     </row>
     <row r="17" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A17" s="8"/>
       <c r="B17" s="8"/>
       <c r="C17" s="16"/>
       <c r="D17" s="16"/>
-      <c r="E17" s="16"/>
-      <c r="F17" s="16"/>
-      <c r="G17" s="28"/>
-      <c r="H17" s="29"/>
-      <c r="I17" s="29"/>
-      <c r="J17" s="30"/>
-      <c r="K17" s="16"/>
-      <c r="L17" s="16"/>
+      <c r="E17" s="17"/>
+      <c r="F17" s="17"/>
+      <c r="G17" s="21"/>
+      <c r="H17" s="22"/>
+      <c r="I17" s="22"/>
+      <c r="J17" s="23"/>
+      <c r="K17" s="24"/>
+      <c r="L17" s="24"/>
     </row>
     <row r="18" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A18" s="5" t="s">
+      <c r="A18" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="B18" s="8"/>
+      <c r="C18" s="16"/>
+      <c r="D18" s="16"/>
+      <c r="E18" s="16"/>
+      <c r="F18" s="16"/>
+      <c r="G18" s="25"/>
+      <c r="H18" s="26"/>
+      <c r="I18" s="26"/>
+      <c r="J18" s="27"/>
+      <c r="K18" s="16"/>
+      <c r="L18" s="16"/>
+    </row>
+    <row r="19" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A19" s="8"/>
+      <c r="B19" s="8"/>
+      <c r="C19" s="16"/>
+      <c r="D19" s="16"/>
+      <c r="E19" s="16"/>
+      <c r="F19" s="16"/>
+      <c r="G19" s="28"/>
+      <c r="H19" s="29"/>
+      <c r="I19" s="29"/>
+      <c r="J19" s="30"/>
+      <c r="K19" s="16"/>
+      <c r="L19" s="16"/>
+    </row>
+    <row r="20" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A20" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="B18" s="6"/>
-      <c r="C18" s="6"/>
-      <c r="D18" s="6"/>
-      <c r="E18" s="6"/>
-      <c r="F18" s="6"/>
-      <c r="G18" s="6"/>
-      <c r="H18" s="6"/>
-      <c r="I18" s="6"/>
-      <c r="J18" s="6"/>
-      <c r="K18" s="6"/>
-      <c r="L18" s="7"/>
-    </row>
-    <row r="19" spans="1:12" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="8" t="s">
+      <c r="B20" s="6"/>
+      <c r="C20" s="6"/>
+      <c r="D20" s="6"/>
+      <c r="E20" s="6"/>
+      <c r="F20" s="6"/>
+      <c r="G20" s="6"/>
+      <c r="H20" s="6"/>
+      <c r="I20" s="6"/>
+      <c r="J20" s="6"/>
+      <c r="K20" s="6"/>
+      <c r="L20" s="7"/>
+    </row>
+    <row r="21" spans="1:12" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A21" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="B19" s="8"/>
-      <c r="C19" s="56" t="s">
+      <c r="B21" s="8"/>
+      <c r="C21" s="55" t="s">
         <v>21</v>
       </c>
-      <c r="D19" s="57"/>
-      <c r="E19" s="10" t="s">
+      <c r="D21" s="56"/>
+      <c r="E21" s="10" t="s">
         <v>22</v>
       </c>
-      <c r="F19" s="12"/>
-      <c r="G19" s="56" t="s">
+      <c r="F21" s="12"/>
+      <c r="G21" s="55" t="s">
         <v>23</v>
       </c>
-      <c r="H19" s="57"/>
-      <c r="I19" s="60" t="s">
+      <c r="H21" s="56"/>
+      <c r="I21" s="59" t="s">
         <v>24</v>
       </c>
-      <c r="J19" s="60" t="s">
+      <c r="J21" s="59" t="s">
         <v>49</v>
       </c>
-      <c r="K19" s="62"/>
-      <c r="L19" s="63"/>
-    </row>
-    <row r="20" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A20" s="8"/>
-      <c r="B20" s="8"/>
-      <c r="C20" s="58"/>
-      <c r="D20" s="59"/>
-      <c r="E20" s="13"/>
-      <c r="F20" s="15"/>
-      <c r="G20" s="58"/>
-      <c r="H20" s="59"/>
-      <c r="I20" s="61"/>
-      <c r="J20" s="61"/>
-      <c r="K20" s="64"/>
-      <c r="L20" s="65"/>
-    </row>
-    <row r="21" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A21" s="8" t="s">
-        <v>25</v>
-      </c>
-      <c r="B21" s="8"/>
-      <c r="C21" s="37"/>
-      <c r="D21" s="38"/>
-      <c r="E21" s="43"/>
-      <c r="F21" s="44"/>
-      <c r="G21" s="43"/>
-      <c r="H21" s="44"/>
-      <c r="I21" s="49"/>
-      <c r="J21" s="52" t="s">
-        <v>50</v>
-      </c>
-      <c r="K21" s="32"/>
-      <c r="L21" s="33"/>
+      <c r="K21" s="61"/>
+      <c r="L21" s="62"/>
     </row>
     <row r="22" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A22" s="8"/>
       <c r="B22" s="8"/>
-      <c r="C22" s="39"/>
-      <c r="D22" s="40"/>
-      <c r="E22" s="45"/>
-      <c r="F22" s="46"/>
-      <c r="G22" s="45"/>
-      <c r="H22" s="46"/>
-      <c r="I22" s="50"/>
-      <c r="J22" s="53"/>
-      <c r="K22" s="54"/>
-      <c r="L22" s="55"/>
+      <c r="C22" s="57"/>
+      <c r="D22" s="58"/>
+      <c r="E22" s="13"/>
+      <c r="F22" s="15"/>
+      <c r="G22" s="57"/>
+      <c r="H22" s="58"/>
+      <c r="I22" s="60"/>
+      <c r="J22" s="60"/>
+      <c r="K22" s="63"/>
+      <c r="L22" s="64"/>
     </row>
     <row r="23" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A23" s="8"/>
+      <c r="A23" s="8" t="s">
+        <v>25</v>
+      </c>
       <c r="B23" s="8"/>
-      <c r="C23" s="41"/>
-      <c r="D23" s="42"/>
-      <c r="E23" s="47"/>
-      <c r="F23" s="48"/>
-      <c r="G23" s="47"/>
-      <c r="H23" s="48"/>
-      <c r="I23" s="51"/>
-      <c r="J23" s="34"/>
-      <c r="K23" s="35"/>
-      <c r="L23" s="36"/>
+      <c r="C23" s="31"/>
+      <c r="D23" s="32"/>
+      <c r="E23" s="37"/>
+      <c r="F23" s="38"/>
+      <c r="G23" s="37"/>
+      <c r="H23" s="38"/>
+      <c r="I23" s="43"/>
+      <c r="J23" s="46" t="s">
+        <v>50</v>
+      </c>
+      <c r="K23" s="47"/>
+      <c r="L23" s="48"/>
     </row>
     <row r="24" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A24" s="8" t="s">
-        <v>26</v>
-      </c>
+      <c r="A24" s="8"/>
       <c r="B24" s="8"/>
-      <c r="C24" s="37"/>
-      <c r="D24" s="38"/>
-      <c r="E24" s="43"/>
-      <c r="F24" s="44"/>
-      <c r="G24" s="43"/>
-      <c r="H24" s="44"/>
-      <c r="I24" s="49"/>
-      <c r="J24" s="52" t="s">
-        <v>50</v>
-      </c>
-      <c r="K24" s="32"/>
-      <c r="L24" s="33"/>
+      <c r="C24" s="33"/>
+      <c r="D24" s="34"/>
+      <c r="E24" s="39"/>
+      <c r="F24" s="40"/>
+      <c r="G24" s="39"/>
+      <c r="H24" s="40"/>
+      <c r="I24" s="44"/>
+      <c r="J24" s="49"/>
+      <c r="K24" s="50"/>
+      <c r="L24" s="51"/>
     </row>
     <row r="25" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A25" s="8"/>
       <c r="B25" s="8"/>
-      <c r="C25" s="39"/>
-      <c r="D25" s="40"/>
-      <c r="E25" s="45"/>
-      <c r="F25" s="46"/>
-      <c r="G25" s="45"/>
-      <c r="H25" s="46"/>
-      <c r="I25" s="50"/>
-      <c r="J25" s="53"/>
-      <c r="K25" s="54"/>
-      <c r="L25" s="55"/>
+      <c r="C25" s="35"/>
+      <c r="D25" s="36"/>
+      <c r="E25" s="41"/>
+      <c r="F25" s="42"/>
+      <c r="G25" s="41"/>
+      <c r="H25" s="42"/>
+      <c r="I25" s="45"/>
+      <c r="J25" s="52"/>
+      <c r="K25" s="53"/>
+      <c r="L25" s="54"/>
     </row>
     <row r="26" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A26" s="8"/>
+      <c r="A26" s="8" t="s">
+        <v>26</v>
+      </c>
       <c r="B26" s="8"/>
-      <c r="C26" s="41"/>
-      <c r="D26" s="42"/>
-      <c r="E26" s="47"/>
-      <c r="F26" s="48"/>
-      <c r="G26" s="47"/>
-      <c r="H26" s="48"/>
-      <c r="I26" s="51"/>
-      <c r="J26" s="34"/>
-      <c r="K26" s="35"/>
-      <c r="L26" s="36"/>
+      <c r="C26" s="31"/>
+      <c r="D26" s="32"/>
+      <c r="E26" s="37"/>
+      <c r="F26" s="38"/>
+      <c r="G26" s="37"/>
+      <c r="H26" s="38"/>
+      <c r="I26" s="43"/>
+      <c r="J26" s="46" t="s">
+        <v>50</v>
+      </c>
+      <c r="K26" s="47"/>
+      <c r="L26" s="48"/>
     </row>
     <row r="27" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A27" s="8" t="s">
-        <v>27</v>
-      </c>
+      <c r="A27" s="8"/>
       <c r="B27" s="8"/>
-      <c r="C27" s="37"/>
-      <c r="D27" s="38"/>
-      <c r="E27" s="43"/>
-      <c r="F27" s="44"/>
-      <c r="G27" s="43"/>
-      <c r="H27" s="44"/>
-      <c r="I27" s="49"/>
-      <c r="J27" s="31"/>
-      <c r="K27" s="32"/>
-      <c r="L27" s="33"/>
+      <c r="C27" s="33"/>
+      <c r="D27" s="34"/>
+      <c r="E27" s="39"/>
+      <c r="F27" s="40"/>
+      <c r="G27" s="39"/>
+      <c r="H27" s="40"/>
+      <c r="I27" s="44"/>
+      <c r="J27" s="49"/>
+      <c r="K27" s="50"/>
+      <c r="L27" s="51"/>
     </row>
     <row r="28" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A28" s="8"/>
       <c r="B28" s="8"/>
-      <c r="C28" s="41"/>
-      <c r="D28" s="42"/>
-      <c r="E28" s="47"/>
-      <c r="F28" s="48"/>
-      <c r="G28" s="47"/>
-      <c r="H28" s="48"/>
-      <c r="I28" s="51"/>
-      <c r="J28" s="34"/>
-      <c r="K28" s="35"/>
-      <c r="L28" s="36"/>
+      <c r="C28" s="35"/>
+      <c r="D28" s="36"/>
+      <c r="E28" s="41"/>
+      <c r="F28" s="42"/>
+      <c r="G28" s="41"/>
+      <c r="H28" s="42"/>
+      <c r="I28" s="45"/>
+      <c r="J28" s="52"/>
+      <c r="K28" s="53"/>
+      <c r="L28" s="54"/>
     </row>
     <row r="29" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A29" s="8" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B29" s="8"/>
-      <c r="C29" s="37"/>
-      <c r="D29" s="38"/>
-      <c r="E29" s="43"/>
-      <c r="F29" s="44"/>
-      <c r="G29" s="43"/>
-      <c r="H29" s="44"/>
-      <c r="I29" s="49"/>
-      <c r="J29" s="31"/>
-      <c r="K29" s="32"/>
-      <c r="L29" s="33"/>
+      <c r="C29" s="31"/>
+      <c r="D29" s="32"/>
+      <c r="E29" s="37"/>
+      <c r="F29" s="38"/>
+      <c r="G29" s="37"/>
+      <c r="H29" s="38"/>
+      <c r="I29" s="43"/>
+      <c r="J29" s="65"/>
+      <c r="K29" s="47"/>
+      <c r="L29" s="48"/>
     </row>
     <row r="30" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A30" s="8"/>
       <c r="B30" s="8"/>
-      <c r="C30" s="41"/>
-      <c r="D30" s="42"/>
-      <c r="E30" s="47"/>
-      <c r="F30" s="48"/>
-      <c r="G30" s="47"/>
-      <c r="H30" s="48"/>
-      <c r="I30" s="51"/>
-      <c r="J30" s="34"/>
-      <c r="K30" s="35"/>
-      <c r="L30" s="36"/>
+      <c r="C30" s="35"/>
+      <c r="D30" s="36"/>
+      <c r="E30" s="41"/>
+      <c r="F30" s="42"/>
+      <c r="G30" s="41"/>
+      <c r="H30" s="42"/>
+      <c r="I30" s="45"/>
+      <c r="J30" s="52"/>
+      <c r="K30" s="53"/>
+      <c r="L30" s="54"/>
     </row>
     <row r="31" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A31" s="5" t="s">
+      <c r="A31" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="B31" s="8"/>
+      <c r="C31" s="31"/>
+      <c r="D31" s="32"/>
+      <c r="E31" s="37"/>
+      <c r="F31" s="38"/>
+      <c r="G31" s="37"/>
+      <c r="H31" s="38"/>
+      <c r="I31" s="43"/>
+      <c r="J31" s="65"/>
+      <c r="K31" s="47"/>
+      <c r="L31" s="48"/>
+    </row>
+    <row r="32" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A32" s="8"/>
+      <c r="B32" s="8"/>
+      <c r="C32" s="35"/>
+      <c r="D32" s="36"/>
+      <c r="E32" s="41"/>
+      <c r="F32" s="42"/>
+      <c r="G32" s="41"/>
+      <c r="H32" s="42"/>
+      <c r="I32" s="45"/>
+      <c r="J32" s="52"/>
+      <c r="K32" s="53"/>
+      <c r="L32" s="54"/>
+    </row>
+    <row r="33" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A33" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="B31" s="6"/>
-      <c r="C31" s="6"/>
-      <c r="D31" s="6"/>
-      <c r="E31" s="6"/>
-      <c r="F31" s="6"/>
-      <c r="G31" s="6"/>
-      <c r="H31" s="6"/>
-      <c r="I31" s="6"/>
-      <c r="J31" s="6"/>
-      <c r="K31" s="6"/>
-      <c r="L31" s="7"/>
-    </row>
-    <row r="32" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A32" s="56" t="s">
+      <c r="B33" s="6"/>
+      <c r="C33" s="6"/>
+      <c r="D33" s="6"/>
+      <c r="E33" s="6"/>
+      <c r="F33" s="6"/>
+      <c r="G33" s="6"/>
+      <c r="H33" s="6"/>
+      <c r="I33" s="6"/>
+      <c r="J33" s="6"/>
+      <c r="K33" s="6"/>
+      <c r="L33" s="7"/>
+    </row>
+    <row r="34" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A34" s="55" t="s">
         <v>13</v>
       </c>
-      <c r="B32" s="57"/>
-      <c r="C32" s="56" t="s">
+      <c r="B34" s="56"/>
+      <c r="C34" s="55" t="s">
         <v>30</v>
       </c>
-      <c r="D32" s="57"/>
-      <c r="E32" s="10" t="s">
+      <c r="D34" s="56"/>
+      <c r="E34" s="10" t="s">
         <v>31</v>
       </c>
-      <c r="F32" s="12"/>
-      <c r="G32" s="56" t="s">
+      <c r="F34" s="12"/>
+      <c r="G34" s="55" t="s">
         <v>32</v>
       </c>
-      <c r="H32" s="57"/>
-      <c r="I32" s="10" t="s">
+      <c r="H34" s="56"/>
+      <c r="I34" s="10" t="s">
         <v>33</v>
       </c>
-      <c r="J32" s="12"/>
-      <c r="K32" s="56" t="s">
+      <c r="J34" s="12"/>
+      <c r="K34" s="55" t="s">
         <v>34</v>
       </c>
-      <c r="L32" s="57"/>
-    </row>
-    <row r="33" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A33" s="58"/>
-      <c r="B33" s="59"/>
-      <c r="C33" s="58"/>
-      <c r="D33" s="59"/>
-      <c r="E33" s="13"/>
-      <c r="F33" s="15"/>
-      <c r="G33" s="58"/>
-      <c r="H33" s="59"/>
-      <c r="I33" s="13"/>
-      <c r="J33" s="15"/>
-      <c r="K33" s="58"/>
-      <c r="L33" s="59"/>
-    </row>
-    <row r="34" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A34" s="56" t="s">
+      <c r="L34" s="56"/>
+    </row>
+    <row r="35" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A35" s="57"/>
+      <c r="B35" s="58"/>
+      <c r="C35" s="57"/>
+      <c r="D35" s="58"/>
+      <c r="E35" s="13"/>
+      <c r="F35" s="15"/>
+      <c r="G35" s="57"/>
+      <c r="H35" s="58"/>
+      <c r="I35" s="13"/>
+      <c r="J35" s="15"/>
+      <c r="K35" s="57"/>
+      <c r="L35" s="58"/>
+    </row>
+    <row r="36" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A36" s="55" t="s">
         <v>25</v>
       </c>
-      <c r="B34" s="57"/>
-      <c r="C34" s="49"/>
-      <c r="D34" s="66"/>
-      <c r="E34" s="43"/>
-      <c r="F34" s="44"/>
-      <c r="G34" s="49"/>
-      <c r="H34" s="66"/>
-      <c r="I34" s="43"/>
-      <c r="J34" s="44"/>
-      <c r="K34" s="49"/>
-      <c r="L34" s="66"/>
-    </row>
-    <row r="35" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A35" s="58"/>
-      <c r="B35" s="59"/>
-      <c r="C35" s="51"/>
-      <c r="D35" s="67"/>
-      <c r="E35" s="47"/>
-      <c r="F35" s="48"/>
-      <c r="G35" s="51"/>
-      <c r="H35" s="67"/>
-      <c r="I35" s="47"/>
-      <c r="J35" s="48"/>
-      <c r="K35" s="51"/>
-      <c r="L35" s="67"/>
-    </row>
-    <row r="36" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A36" s="56" t="s">
+      <c r="B36" s="56"/>
+      <c r="C36" s="43"/>
+      <c r="D36" s="66"/>
+      <c r="E36" s="37"/>
+      <c r="F36" s="38"/>
+      <c r="G36" s="43"/>
+      <c r="H36" s="66"/>
+      <c r="I36" s="37"/>
+      <c r="J36" s="38"/>
+      <c r="K36" s="43"/>
+      <c r="L36" s="66"/>
+    </row>
+    <row r="37" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A37" s="57"/>
+      <c r="B37" s="58"/>
+      <c r="C37" s="45"/>
+      <c r="D37" s="67"/>
+      <c r="E37" s="41"/>
+      <c r="F37" s="42"/>
+      <c r="G37" s="45"/>
+      <c r="H37" s="67"/>
+      <c r="I37" s="41"/>
+      <c r="J37" s="42"/>
+      <c r="K37" s="45"/>
+      <c r="L37" s="67"/>
+    </row>
+    <row r="38" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A38" s="55" t="s">
         <v>26</v>
       </c>
-      <c r="B36" s="57"/>
-      <c r="C36" s="49"/>
-      <c r="D36" s="66"/>
-      <c r="E36" s="43"/>
-      <c r="F36" s="44"/>
-      <c r="G36" s="49"/>
-      <c r="H36" s="66"/>
-      <c r="I36" s="43"/>
-      <c r="J36" s="44"/>
-      <c r="K36" s="49"/>
-      <c r="L36" s="66"/>
-    </row>
-    <row r="37" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A37" s="58"/>
-      <c r="B37" s="59"/>
-      <c r="C37" s="51"/>
-      <c r="D37" s="67"/>
-      <c r="E37" s="47"/>
-      <c r="F37" s="48"/>
-      <c r="G37" s="51"/>
-      <c r="H37" s="67"/>
-      <c r="I37" s="47"/>
-      <c r="J37" s="48"/>
-      <c r="K37" s="51"/>
-      <c r="L37" s="67"/>
-    </row>
-    <row r="38" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A38" s="56" t="s">
+      <c r="B38" s="56"/>
+      <c r="C38" s="43"/>
+      <c r="D38" s="66"/>
+      <c r="E38" s="37"/>
+      <c r="F38" s="38"/>
+      <c r="G38" s="43"/>
+      <c r="H38" s="66"/>
+      <c r="I38" s="37"/>
+      <c r="J38" s="38"/>
+      <c r="K38" s="43"/>
+      <c r="L38" s="66"/>
+    </row>
+    <row r="39" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A39" s="57"/>
+      <c r="B39" s="58"/>
+      <c r="C39" s="45"/>
+      <c r="D39" s="67"/>
+      <c r="E39" s="41"/>
+      <c r="F39" s="42"/>
+      <c r="G39" s="45"/>
+      <c r="H39" s="67"/>
+      <c r="I39" s="41"/>
+      <c r="J39" s="42"/>
+      <c r="K39" s="45"/>
+      <c r="L39" s="67"/>
+    </row>
+    <row r="40" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A40" s="55" t="s">
         <v>35</v>
       </c>
-      <c r="B38" s="57"/>
-      <c r="C38" s="9" t="s">
+      <c r="B40" s="56"/>
+      <c r="C40" s="9" t="s">
         <v>36</v>
       </c>
-      <c r="D38" s="9"/>
-      <c r="E38" s="9" t="s">
+      <c r="D40" s="9"/>
+      <c r="E40" s="9" t="s">
         <v>37</v>
       </c>
-      <c r="F38" s="9"/>
-      <c r="G38" s="9" t="s">
+      <c r="F40" s="9"/>
+      <c r="G40" s="9" t="s">
         <v>28</v>
       </c>
-      <c r="H38" s="9"/>
-      <c r="I38" s="70" t="s">
+      <c r="H40" s="9"/>
+      <c r="I40" s="70" t="s">
         <v>38</v>
       </c>
-      <c r="J38" s="70"/>
-      <c r="K38" s="71" t="s">
+      <c r="J40" s="70"/>
+      <c r="K40" s="71" t="s">
         <v>39</v>
       </c>
-      <c r="L38" s="72"/>
-    </row>
-    <row r="39" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A39" s="58"/>
-      <c r="B39" s="59"/>
-      <c r="C39" s="75"/>
-      <c r="D39" s="76"/>
-      <c r="E39" s="77"/>
-      <c r="F39" s="78"/>
-      <c r="G39" s="9"/>
-      <c r="H39" s="9"/>
-      <c r="I39" s="79"/>
-      <c r="J39" s="80"/>
-      <c r="K39" s="73"/>
-      <c r="L39" s="74"/>
-    </row>
-    <row r="40" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A40" s="5" t="s">
+      <c r="L40" s="72"/>
+    </row>
+    <row r="41" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A41" s="57"/>
+      <c r="B41" s="58"/>
+      <c r="C41" s="75"/>
+      <c r="D41" s="76"/>
+      <c r="E41" s="77"/>
+      <c r="F41" s="78"/>
+      <c r="G41" s="9"/>
+      <c r="H41" s="9"/>
+      <c r="I41" s="79"/>
+      <c r="J41" s="80"/>
+      <c r="K41" s="73"/>
+      <c r="L41" s="74"/>
+    </row>
+    <row r="42" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A42" s="5" t="s">
         <v>40</v>
       </c>
-      <c r="B40" s="6"/>
-      <c r="C40" s="6"/>
-      <c r="D40" s="6"/>
-      <c r="E40" s="6"/>
-      <c r="F40" s="6"/>
-      <c r="G40" s="6"/>
-      <c r="H40" s="6"/>
-      <c r="I40" s="6"/>
-      <c r="J40" s="6"/>
-      <c r="K40" s="6"/>
-      <c r="L40" s="7"/>
-    </row>
-    <row r="41" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A41" s="17" t="s">
+      <c r="B42" s="6"/>
+      <c r="C42" s="6"/>
+      <c r="D42" s="6"/>
+      <c r="E42" s="6"/>
+      <c r="F42" s="6"/>
+      <c r="G42" s="6"/>
+      <c r="H42" s="6"/>
+      <c r="I42" s="6"/>
+      <c r="J42" s="6"/>
+      <c r="K42" s="6"/>
+      <c r="L42" s="7"/>
+    </row>
+    <row r="43" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A43" s="17" t="s">
         <v>41</v>
       </c>
-      <c r="B41" s="17"/>
-      <c r="C41" s="68" t="s">
+      <c r="B43" s="17"/>
+      <c r="C43" s="68" t="s">
         <v>52</v>
       </c>
-      <c r="D41" s="69"/>
-      <c r="E41" s="17" t="s">
+      <c r="D43" s="69"/>
+      <c r="E43" s="17" t="s">
         <v>42</v>
       </c>
-      <c r="F41" s="17"/>
-      <c r="G41" s="69"/>
-      <c r="H41" s="69"/>
-      <c r="I41" s="17" t="s">
+      <c r="F43" s="17"/>
+      <c r="G43" s="69"/>
+      <c r="H43" s="69"/>
+      <c r="I43" s="17" t="s">
         <v>43</v>
       </c>
-      <c r="J41" s="17"/>
-      <c r="K41" s="68" t="s">
+      <c r="J43" s="17"/>
+      <c r="K43" s="68" t="s">
         <v>54</v>
       </c>
-      <c r="L41" s="69"/>
-    </row>
-    <row r="42" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A42" s="17"/>
-      <c r="B42" s="17"/>
-      <c r="C42" s="69"/>
-      <c r="D42" s="69"/>
-      <c r="E42" s="17"/>
-      <c r="F42" s="17"/>
-      <c r="G42" s="69"/>
-      <c r="H42" s="69"/>
-      <c r="I42" s="17"/>
-      <c r="J42" s="17"/>
-      <c r="K42" s="69"/>
-      <c r="L42" s="69"/>
-    </row>
-    <row r="43" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A43" s="5" t="s">
+      <c r="L43" s="69"/>
+    </row>
+    <row r="44" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A44" s="17"/>
+      <c r="B44" s="17"/>
+      <c r="C44" s="69"/>
+      <c r="D44" s="69"/>
+      <c r="E44" s="17"/>
+      <c r="F44" s="17"/>
+      <c r="G44" s="69"/>
+      <c r="H44" s="69"/>
+      <c r="I44" s="17"/>
+      <c r="J44" s="17"/>
+      <c r="K44" s="69"/>
+      <c r="L44" s="69"/>
+    </row>
+    <row r="45" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A45" s="5" t="s">
         <v>44</v>
       </c>
-      <c r="B43" s="6"/>
-      <c r="C43" s="6"/>
-      <c r="D43" s="6"/>
-      <c r="E43" s="6"/>
-      <c r="F43" s="6"/>
-      <c r="G43" s="6"/>
-      <c r="H43" s="6"/>
-      <c r="I43" s="6"/>
-      <c r="J43" s="6"/>
-      <c r="K43" s="6"/>
-      <c r="L43" s="7"/>
-    </row>
-    <row r="44" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A44" s="17" t="s">
+      <c r="B45" s="6"/>
+      <c r="C45" s="6"/>
+      <c r="D45" s="6"/>
+      <c r="E45" s="6"/>
+      <c r="F45" s="6"/>
+      <c r="G45" s="6"/>
+      <c r="H45" s="6"/>
+      <c r="I45" s="6"/>
+      <c r="J45" s="6"/>
+      <c r="K45" s="6"/>
+      <c r="L45" s="7"/>
+    </row>
+    <row r="46" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A46" s="17" t="s">
         <v>45</v>
       </c>
-      <c r="B44" s="17"/>
-      <c r="C44" s="69" t="s">
+      <c r="B46" s="17"/>
+      <c r="C46" s="69" t="s">
         <v>51</v>
       </c>
-      <c r="D44" s="69"/>
-      <c r="E44" s="17" t="s">
+      <c r="D46" s="69"/>
+      <c r="E46" s="17" t="s">
         <v>46</v>
       </c>
-      <c r="F44" s="17"/>
-      <c r="G44" s="69" t="s">
+      <c r="F46" s="17"/>
+      <c r="G46" s="69" t="s">
         <v>52</v>
       </c>
-      <c r="H44" s="69"/>
-      <c r="I44" s="17" t="s">
+      <c r="H46" s="69"/>
+      <c r="I46" s="17" t="s">
         <v>47</v>
       </c>
-      <c r="J44" s="17"/>
-      <c r="K44" s="69" t="s">
+      <c r="J46" s="17"/>
+      <c r="K46" s="69" t="s">
         <v>53</v>
       </c>
-      <c r="L44" s="69"/>
-    </row>
-    <row r="45" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A45" s="17"/>
-      <c r="B45" s="17"/>
-      <c r="C45" s="69"/>
-      <c r="D45" s="69"/>
-      <c r="E45" s="17"/>
-      <c r="F45" s="17"/>
-      <c r="G45" s="69"/>
-      <c r="H45" s="69"/>
-      <c r="I45" s="17"/>
-      <c r="J45" s="17"/>
-      <c r="K45" s="69"/>
-      <c r="L45" s="69"/>
-    </row>
-    <row r="46" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A46" s="5" t="s">
+      <c r="L46" s="69"/>
+    </row>
+    <row r="47" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A47" s="17"/>
+      <c r="B47" s="17"/>
+      <c r="C47" s="69"/>
+      <c r="D47" s="69"/>
+      <c r="E47" s="17"/>
+      <c r="F47" s="17"/>
+      <c r="G47" s="69"/>
+      <c r="H47" s="69"/>
+      <c r="I47" s="17"/>
+      <c r="J47" s="17"/>
+      <c r="K47" s="69"/>
+      <c r="L47" s="69"/>
+    </row>
+    <row r="48" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A48" s="5" t="s">
         <v>48</v>
       </c>
-      <c r="B46" s="6"/>
-      <c r="C46" s="6"/>
-      <c r="D46" s="6"/>
-      <c r="E46" s="6"/>
-      <c r="F46" s="6"/>
-      <c r="G46" s="6"/>
-      <c r="H46" s="6"/>
-      <c r="I46" s="6"/>
-      <c r="J46" s="6"/>
-      <c r="K46" s="6"/>
-      <c r="L46" s="7"/>
-    </row>
-    <row r="47" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A47" s="81"/>
-      <c r="B47" s="82"/>
-      <c r="C47" s="82"/>
-      <c r="D47" s="82"/>
-      <c r="E47" s="82"/>
-      <c r="F47" s="82"/>
-      <c r="G47" s="82"/>
-      <c r="H47" s="82"/>
-      <c r="I47" s="82"/>
-      <c r="J47" s="82"/>
-      <c r="K47" s="82"/>
-      <c r="L47" s="83"/>
-    </row>
-    <row r="48" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A48" s="84"/>
-      <c r="B48" s="85"/>
-      <c r="C48" s="85"/>
-      <c r="D48" s="85"/>
-      <c r="E48" s="85"/>
-      <c r="F48" s="85"/>
-      <c r="G48" s="85"/>
-      <c r="H48" s="85"/>
-      <c r="I48" s="85"/>
-      <c r="J48" s="85"/>
-      <c r="K48" s="85"/>
-      <c r="L48" s="86"/>
+      <c r="B48" s="6"/>
+      <c r="C48" s="6"/>
+      <c r="D48" s="6"/>
+      <c r="E48" s="6"/>
+      <c r="F48" s="6"/>
+      <c r="G48" s="6"/>
+      <c r="H48" s="6"/>
+      <c r="I48" s="6"/>
+      <c r="J48" s="6"/>
+      <c r="K48" s="6"/>
+      <c r="L48" s="7"/>
     </row>
     <row r="49" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A49" s="84"/>
-      <c r="B49" s="85"/>
-      <c r="C49" s="85"/>
-      <c r="D49" s="85"/>
-      <c r="E49" s="85"/>
-      <c r="F49" s="85"/>
-      <c r="G49" s="85"/>
-      <c r="H49" s="85"/>
-      <c r="I49" s="85"/>
-      <c r="J49" s="85"/>
-      <c r="K49" s="85"/>
-      <c r="L49" s="86"/>
+      <c r="A49" s="81"/>
+      <c r="B49" s="82"/>
+      <c r="C49" s="82"/>
+      <c r="D49" s="82"/>
+      <c r="E49" s="82"/>
+      <c r="F49" s="82"/>
+      <c r="G49" s="82"/>
+      <c r="H49" s="82"/>
+      <c r="I49" s="82"/>
+      <c r="J49" s="82"/>
+      <c r="K49" s="82"/>
+      <c r="L49" s="83"/>
     </row>
     <row r="50" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A50" s="84"/>
@@ -2023,101 +2031,134 @@
       <c r="L52" s="86"/>
     </row>
     <row r="53" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A53" s="87"/>
-      <c r="B53" s="88"/>
-      <c r="C53" s="88"/>
-      <c r="D53" s="88"/>
-      <c r="E53" s="88"/>
-      <c r="F53" s="88"/>
-      <c r="G53" s="88"/>
-      <c r="H53" s="88"/>
-      <c r="I53" s="88"/>
-      <c r="J53" s="88"/>
-      <c r="K53" s="88"/>
-      <c r="L53" s="89"/>
+      <c r="A53" s="84"/>
+      <c r="B53" s="85"/>
+      <c r="C53" s="85"/>
+      <c r="D53" s="85"/>
+      <c r="E53" s="85"/>
+      <c r="F53" s="85"/>
+      <c r="G53" s="85"/>
+      <c r="H53" s="85"/>
+      <c r="I53" s="85"/>
+      <c r="J53" s="85"/>
+      <c r="K53" s="85"/>
+      <c r="L53" s="86"/>
+    </row>
+    <row r="54" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A54" s="84"/>
+      <c r="B54" s="85"/>
+      <c r="C54" s="85"/>
+      <c r="D54" s="85"/>
+      <c r="E54" s="85"/>
+      <c r="F54" s="85"/>
+      <c r="G54" s="85"/>
+      <c r="H54" s="85"/>
+      <c r="I54" s="85"/>
+      <c r="J54" s="85"/>
+      <c r="K54" s="85"/>
+      <c r="L54" s="86"/>
+    </row>
+    <row r="55" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A55" s="87"/>
+      <c r="B55" s="88"/>
+      <c r="C55" s="88"/>
+      <c r="D55" s="88"/>
+      <c r="E55" s="88"/>
+      <c r="F55" s="88"/>
+      <c r="G55" s="88"/>
+      <c r="H55" s="88"/>
+      <c r="I55" s="88"/>
+      <c r="J55" s="88"/>
+      <c r="K55" s="88"/>
+      <c r="L55" s="89"/>
     </row>
   </sheetData>
-  <mergeCells count="108">
-    <mergeCell ref="A46:L46"/>
-    <mergeCell ref="A47:L53"/>
-    <mergeCell ref="A43:L43"/>
-    <mergeCell ref="A44:B45"/>
-    <mergeCell ref="C44:D45"/>
-    <mergeCell ref="E44:F45"/>
-    <mergeCell ref="G44:H45"/>
-    <mergeCell ref="I44:J45"/>
-    <mergeCell ref="K44:L45"/>
-    <mergeCell ref="A40:L40"/>
-    <mergeCell ref="A41:B42"/>
-    <mergeCell ref="C41:D42"/>
-    <mergeCell ref="E41:F42"/>
-    <mergeCell ref="G41:H42"/>
-    <mergeCell ref="I41:J42"/>
-    <mergeCell ref="K41:L42"/>
+  <mergeCells count="113">
+    <mergeCell ref="A48:L48"/>
+    <mergeCell ref="A49:L55"/>
+    <mergeCell ref="A45:L45"/>
+    <mergeCell ref="A46:B47"/>
+    <mergeCell ref="C46:D47"/>
+    <mergeCell ref="E46:F47"/>
+    <mergeCell ref="G46:H47"/>
+    <mergeCell ref="I46:J47"/>
+    <mergeCell ref="K46:L47"/>
+    <mergeCell ref="A42:L42"/>
+    <mergeCell ref="A43:B44"/>
+    <mergeCell ref="C43:D44"/>
+    <mergeCell ref="E43:F44"/>
+    <mergeCell ref="G43:H44"/>
+    <mergeCell ref="I43:J44"/>
+    <mergeCell ref="K43:L44"/>
+    <mergeCell ref="A40:B41"/>
+    <mergeCell ref="C40:D40"/>
+    <mergeCell ref="E40:F40"/>
+    <mergeCell ref="G40:H41"/>
+    <mergeCell ref="I40:J40"/>
+    <mergeCell ref="K40:L41"/>
+    <mergeCell ref="C41:D41"/>
+    <mergeCell ref="E41:F41"/>
+    <mergeCell ref="I41:J41"/>
+    <mergeCell ref="J29:L30"/>
+    <mergeCell ref="A29:B30"/>
+    <mergeCell ref="C29:D30"/>
+    <mergeCell ref="E29:F30"/>
+    <mergeCell ref="G29:H30"/>
+    <mergeCell ref="I29:I30"/>
     <mergeCell ref="A38:B39"/>
-    <mergeCell ref="C38:D38"/>
-    <mergeCell ref="E38:F38"/>
+    <mergeCell ref="C38:D39"/>
+    <mergeCell ref="E38:F39"/>
     <mergeCell ref="G38:H39"/>
-    <mergeCell ref="I38:J38"/>
+    <mergeCell ref="I38:J39"/>
     <mergeCell ref="K38:L39"/>
-    <mergeCell ref="C39:D39"/>
-    <mergeCell ref="E39:F39"/>
-    <mergeCell ref="I39:J39"/>
     <mergeCell ref="A36:B37"/>
     <mergeCell ref="C36:D37"/>
     <mergeCell ref="E36:F37"/>
     <mergeCell ref="G36:H37"/>
     <mergeCell ref="I36:J37"/>
     <mergeCell ref="K36:L37"/>
+    <mergeCell ref="A33:L33"/>
     <mergeCell ref="A34:B35"/>
     <mergeCell ref="C34:D35"/>
     <mergeCell ref="E34:F35"/>
     <mergeCell ref="G34:H35"/>
     <mergeCell ref="I34:J35"/>
     <mergeCell ref="K34:L35"/>
-    <mergeCell ref="I24:I26"/>
-    <mergeCell ref="A31:L31"/>
-    <mergeCell ref="A32:B33"/>
-    <mergeCell ref="C32:D33"/>
-    <mergeCell ref="E32:F33"/>
-    <mergeCell ref="G32:H33"/>
-    <mergeCell ref="I32:J33"/>
-    <mergeCell ref="K32:L33"/>
-    <mergeCell ref="A29:B30"/>
-    <mergeCell ref="C29:D30"/>
-    <mergeCell ref="E29:F30"/>
-    <mergeCell ref="G29:H30"/>
-    <mergeCell ref="I29:I30"/>
-    <mergeCell ref="J29:L30"/>
-    <mergeCell ref="J27:L28"/>
-    <mergeCell ref="A21:B23"/>
-    <mergeCell ref="C21:D23"/>
-    <mergeCell ref="E21:F23"/>
-    <mergeCell ref="G21:H23"/>
-    <mergeCell ref="I21:I23"/>
-    <mergeCell ref="J21:L23"/>
-    <mergeCell ref="J24:L26"/>
-    <mergeCell ref="A18:L18"/>
-    <mergeCell ref="A19:B20"/>
-    <mergeCell ref="C19:D20"/>
-    <mergeCell ref="E19:F20"/>
-    <mergeCell ref="G19:H20"/>
-    <mergeCell ref="I19:I20"/>
-    <mergeCell ref="J19:L20"/>
-    <mergeCell ref="A27:B28"/>
-    <mergeCell ref="C27:D28"/>
-    <mergeCell ref="E27:F28"/>
-    <mergeCell ref="G27:H28"/>
-    <mergeCell ref="I27:I28"/>
-    <mergeCell ref="A24:B26"/>
-    <mergeCell ref="C24:D26"/>
-    <mergeCell ref="E24:F26"/>
-    <mergeCell ref="G24:H26"/>
+    <mergeCell ref="A31:B32"/>
+    <mergeCell ref="C31:D32"/>
+    <mergeCell ref="E31:F32"/>
+    <mergeCell ref="G31:H32"/>
+    <mergeCell ref="I31:I32"/>
+    <mergeCell ref="J31:L32"/>
+    <mergeCell ref="A23:B25"/>
+    <mergeCell ref="C23:D25"/>
+    <mergeCell ref="E23:F25"/>
+    <mergeCell ref="G23:H25"/>
+    <mergeCell ref="I23:I25"/>
+    <mergeCell ref="J23:L25"/>
+    <mergeCell ref="J26:L28"/>
+    <mergeCell ref="A20:L20"/>
+    <mergeCell ref="A21:B22"/>
+    <mergeCell ref="C21:D22"/>
+    <mergeCell ref="E21:F22"/>
+    <mergeCell ref="G21:H22"/>
+    <mergeCell ref="I21:I22"/>
+    <mergeCell ref="J21:L22"/>
+    <mergeCell ref="A26:B28"/>
+    <mergeCell ref="C26:D28"/>
+    <mergeCell ref="E26:F28"/>
+    <mergeCell ref="G26:H28"/>
+    <mergeCell ref="I26:I28"/>
     <mergeCell ref="A14:B15"/>
     <mergeCell ref="C14:D15"/>
     <mergeCell ref="E14:F15"/>
     <mergeCell ref="G14:J15"/>
     <mergeCell ref="K14:L15"/>
+    <mergeCell ref="A18:B19"/>
+    <mergeCell ref="C18:D19"/>
+    <mergeCell ref="E18:F19"/>
+    <mergeCell ref="G18:J19"/>
+    <mergeCell ref="K18:L19"/>
     <mergeCell ref="A16:B17"/>
     <mergeCell ref="C16:D17"/>
     <mergeCell ref="E16:F17"/>
@@ -2149,6 +2190,6 @@
   </mergeCells>
   <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" scale="83" orientation="portrait" r:id="rId1"/>
+  <pageSetup paperSize="9" scale="80" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>